<commit_message>
Modification de la source
Signed-off-by: Guillaume Daudin <gdaudin@mac.com>
</commit_message>
<xml_diff>
--- a/Verified multipleformat sources/Local/Nantes/Nantes export 1733 vb.xlsx
+++ b/Verified multipleformat sources/Local/Nantes/Nantes export 1733 vb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumedaudin/Répertoires Git/toflit18_data_GIT/Unverified multiformat sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumedaudin/Répertoires Git/toflit18_data_GIT/Verified multipleformat sources/Local/Nantes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0222F1C-732B-FE43-A1CB-80576D66C494}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEC0388-FA97-3642-B618-5D20B381EE14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="500" windowWidth="25600" windowHeight="16380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5578" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5578" uniqueCount="605">
   <si>
     <t>Nom Marchandise</t>
   </si>
@@ -1716,9 +1716,6 @@
   </si>
   <si>
     <t>mention "ai 9 s." ?</t>
-  </si>
-  <si>
-    <t>Err</t>
   </si>
   <si>
     <t>Le prix a l’air bon, les quantités aussi : la valeur est moins plausible(419500) je l’enlève</t>
@@ -2403,9 +2400,9 @@
   <dimension ref="A1:AB951"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A763" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="V775" sqref="V775"/>
+      <selection pane="bottomLeft" activeCell="V182" sqref="V182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2481,7 +2478,7 @@
         <v>11</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>12</v>
@@ -13737,7 +13734,7 @@
         <v>-2000</v>
       </c>
       <c r="V181" s="8" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
     </row>
     <row r="182" spans="1:22">
@@ -16901,7 +16898,7 @@
       </c>
       <c r="U232" s="18"/>
       <c r="V232" s="8" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="233" spans="1:22">
@@ -18319,7 +18316,7 @@
       </c>
       <c r="U255" s="18"/>
       <c r="V255" s="8" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="256" spans="1:22">
@@ -18985,7 +18982,7 @@
       </c>
       <c r="U266" s="18"/>
       <c r="V266" s="8" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="267" spans="1:22">
@@ -19111,7 +19108,7 @@
         <v>0</v>
       </c>
       <c r="V268" s="8" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="269" spans="1:22">
@@ -19665,7 +19662,7 @@
       </c>
       <c r="U277" s="18"/>
       <c r="V277" s="8" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="278" spans="1:22">
@@ -21369,7 +21366,7 @@
       </c>
       <c r="U304" s="18"/>
       <c r="V304" s="8" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="305" spans="1:25">
@@ -23714,7 +23711,7 @@
       </c>
       <c r="U342" s="18"/>
       <c r="V342" s="8" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="343" spans="1:25">
@@ -23770,7 +23767,7 @@
       </c>
       <c r="U343" s="18"/>
       <c r="V343" s="8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="344" spans="1:25">
@@ -24816,7 +24813,7 @@
       </c>
       <c r="U360" s="18"/>
       <c r="V360" s="8" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="361" spans="1:22">
@@ -26215,7 +26212,7 @@
       <c r="M384" s="13"/>
       <c r="N384" s="15"/>
       <c r="O384" s="16">
-        <f t="shared" ref="O382:O445" si="36">L384+(0.05*M384)+(N384/240)</f>
+        <f t="shared" ref="O384:O445" si="36">L384+(0.05*M384)+(N384/240)</f>
         <v>60</v>
       </c>
       <c r="P384" s="17">
@@ -26228,11 +26225,11 @@
         <v>2100</v>
       </c>
       <c r="T384" s="18">
-        <f t="shared" ref="T382:T445" si="37">J384*O384</f>
+        <f t="shared" ref="T384:T445" si="37">J384*O384</f>
         <v>2100</v>
       </c>
       <c r="U384" s="18">
-        <f t="shared" ref="U382:U445" si="38">S384-T384</f>
+        <f t="shared" ref="U384:U445" si="38">S384-T384</f>
         <v>0</v>
       </c>
       <c r="V384" s="8"/>
@@ -27638,7 +27635,7 @@
       </c>
       <c r="U407" s="18"/>
       <c r="V407" s="8" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="408" spans="1:22">
@@ -27694,7 +27691,7 @@
       </c>
       <c r="U408" s="18"/>
       <c r="V408" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="409" spans="1:22">
@@ -27884,7 +27881,7 @@
         <v>590</v>
       </c>
       <c r="V411" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="412" spans="1:22">
@@ -28844,7 +28841,7 @@
         <v>-2</v>
       </c>
       <c r="V426" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="427" spans="1:25">
@@ -30169,7 +30166,7 @@
         <v>452</v>
       </c>
       <c r="X448" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="Y448">
         <v>3.25</v>
@@ -30900,7 +30897,7 @@
       </c>
       <c r="U460" s="18"/>
       <c r="V460" s="8" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="461" spans="1:22">
@@ -31144,7 +31141,7 @@
       </c>
       <c r="U464" s="18"/>
       <c r="V464" s="8" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="465" spans="1:22">
@@ -31328,7 +31325,7 @@
         <v>0</v>
       </c>
       <c r="V467" s="8" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="468" spans="1:22">
@@ -32186,7 +32183,7 @@
       </c>
       <c r="U481" s="18"/>
       <c r="V481" s="8" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="482" spans="1:25">
@@ -32678,7 +32675,7 @@
         <v>37</v>
       </c>
       <c r="Y489">
-        <f t="shared" ref="Y489:Y490" si="44">49/20</f>
+        <f t="shared" ref="Y489" si="44">49/20</f>
         <v>2.4500000000000002</v>
       </c>
     </row>
@@ -33125,7 +33122,7 @@
         <v>27.5</v>
       </c>
       <c r="X496" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="Y496">
         <v>3.25</v>
@@ -34000,7 +33997,7 @@
       </c>
       <c r="U510" s="18"/>
       <c r="V510" s="8" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="511" spans="1:22">
@@ -34052,7 +34049,7 @@
       <c r="Q511" s="17"/>
       <c r="R511" s="17"/>
       <c r="S511" s="18">
-        <f t="shared" ref="S510:S573" si="47">P511+(Q511*0.05)+(R511/240)</f>
+        <f t="shared" ref="S511:S573" si="47">P511+(Q511*0.05)+(R511/240)</f>
         <v>140</v>
       </c>
       <c r="T511" s="18">
@@ -34060,7 +34057,7 @@
         <v>140</v>
       </c>
       <c r="U511" s="18">
-        <f t="shared" ref="U510:U573" si="48">S511-T511</f>
+        <f t="shared" ref="U511:U573" si="48">S511-T511</f>
         <v>0</v>
       </c>
       <c r="V511" s="8"/>
@@ -34159,7 +34156,7 @@
         <v>5185</v>
       </c>
       <c r="K513" s="14" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="L513" s="13">
         <v>7</v>
@@ -34182,7 +34179,7 @@
       </c>
       <c r="U513" s="18"/>
       <c r="V513" s="8" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="514" spans="1:22">
@@ -34548,7 +34545,7 @@
       </c>
       <c r="U519" s="18"/>
       <c r="V519" s="8" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="520" spans="1:22">
@@ -34786,7 +34783,7 @@
       </c>
       <c r="U523" s="18"/>
       <c r="V523" s="8" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="524" spans="1:22">
@@ -34842,7 +34839,7 @@
       </c>
       <c r="U524" s="18"/>
       <c r="V524" s="8" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="525" spans="1:22">
@@ -35708,7 +35705,7 @@
       </c>
       <c r="U538" s="18"/>
       <c r="V538" s="8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="539" spans="1:22">
@@ -36136,7 +36133,7 @@
       </c>
       <c r="U545" s="18"/>
       <c r="V545" s="8" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="546" spans="1:22">
@@ -37295,7 +37292,7 @@
       </c>
       <c r="U564" s="18"/>
       <c r="V564" s="8" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="565" spans="1:22">
@@ -37603,7 +37600,7 @@
       </c>
       <c r="U569" s="18"/>
       <c r="V569" s="8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="570" spans="1:22">
@@ -37903,7 +37900,7 @@
       <c r="Q574" s="17"/>
       <c r="R574" s="17"/>
       <c r="S574" s="18">
-        <f t="shared" ref="S574:S637" si="50">P574+(Q574*0.05)+(R574/240)</f>
+        <f t="shared" ref="S574:S636" si="50">P574+(Q574*0.05)+(R574/240)</f>
         <v>600</v>
       </c>
       <c r="T574" s="18">
@@ -37911,7 +37908,7 @@
         <v>600</v>
       </c>
       <c r="U574" s="18">
-        <f t="shared" ref="U574:U637" si="52">S574-T574</f>
+        <f t="shared" ref="U574:U635" si="52">S574-T574</f>
         <v>0</v>
       </c>
       <c r="V574" s="8"/>
@@ -38031,7 +38028,7 @@
       </c>
       <c r="U576" s="18"/>
       <c r="V576" s="8" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="577" spans="1:22">
@@ -38604,7 +38601,7 @@
         <v>1733</v>
       </c>
       <c r="G586" s="11" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="H586" s="8" t="s">
         <v>22</v>
@@ -38640,7 +38637,7 @@
         <v>-315</v>
       </c>
       <c r="V586" s="8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="587" spans="1:22">
@@ -39504,7 +39501,7 @@
       </c>
       <c r="U600" s="18"/>
       <c r="V600" s="8" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="601" spans="1:22">
@@ -39560,7 +39557,7 @@
       </c>
       <c r="U601" s="18"/>
       <c r="V601" s="8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="602" spans="1:22">
@@ -39616,7 +39613,7 @@
       </c>
       <c r="U602" s="18"/>
       <c r="V602" s="8" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="603" spans="1:22">
@@ -39736,7 +39733,7 @@
       </c>
       <c r="U604" s="18"/>
       <c r="V604" s="8" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="605" spans="1:22">
@@ -40040,7 +40037,7 @@
       </c>
       <c r="U609" s="18"/>
       <c r="V609" s="8" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="610" spans="1:22">
@@ -41150,7 +41147,7 @@
       </c>
       <c r="U627" s="18"/>
       <c r="V627" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="628" spans="1:22">
@@ -41208,7 +41205,7 @@
       </c>
       <c r="U628" s="18"/>
       <c r="V628" s="8" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="629" spans="1:22">
@@ -41512,7 +41509,7 @@
       </c>
       <c r="U633" s="18"/>
       <c r="V633" s="8" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="634" spans="1:22">
@@ -41743,7 +41740,7 @@
       </c>
       <c r="U637" s="18"/>
       <c r="V637" s="8" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="638" spans="1:22">
@@ -45649,7 +45646,7 @@
         <v>-6</v>
       </c>
       <c r="V702" s="8" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="703" spans="1:22">
@@ -46053,7 +46050,7 @@
       <c r="T709" s="18"/>
       <c r="U709" s="18"/>
       <c r="V709" s="8" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="710" spans="1:23">
@@ -46101,7 +46098,7 @@
       <c r="T710" s="18"/>
       <c r="U710" s="18"/>
       <c r="V710" s="8" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="711" spans="1:23">
@@ -46149,7 +46146,7 @@
       <c r="T711" s="18"/>
       <c r="U711" s="18"/>
       <c r="V711" s="8" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="712" spans="1:23">
@@ -46205,7 +46202,7 @@
       </c>
       <c r="U712" s="18"/>
       <c r="V712" s="8" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="W712" s="25"/>
     </row>
@@ -46300,7 +46297,7 @@
       <c r="T714" s="18"/>
       <c r="U714" s="18"/>
       <c r="V714" s="8" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="715" spans="1:23">
@@ -47277,7 +47274,7 @@
         <v>-1060</v>
       </c>
       <c r="V730" s="8" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="731" spans="1:22">
@@ -48124,7 +48121,7 @@
       <c r="M744" s="13"/>
       <c r="N744" s="15"/>
       <c r="O744" s="16">
-        <f t="shared" ref="O744:O807" si="61">L744+(0.05*M744)+(N744/240)</f>
+        <f t="shared" ref="O744:O782" si="61">L744+(0.05*M744)+(N744/240)</f>
         <v>0.17</v>
       </c>
       <c r="P744" s="17">
@@ -48133,15 +48130,15 @@
       <c r="Q744" s="17"/>
       <c r="R744" s="17"/>
       <c r="S744" s="18">
-        <f t="shared" ref="S744:S807" si="62">P744+(Q744*0.05)+(R744/240)</f>
+        <f t="shared" ref="S744:S782" si="62">P744+(Q744*0.05)+(R744/240)</f>
         <v>454</v>
       </c>
       <c r="T744" s="18">
-        <f t="shared" ref="T744:T807" si="63">J744*O744</f>
+        <f t="shared" ref="T744:T782" si="63">J744*O744</f>
         <v>454.75000000000006</v>
       </c>
       <c r="U744" s="18">
-        <f t="shared" ref="U744:U807" si="64">S744-T744</f>
+        <f t="shared" ref="U744:U782" si="64">S744-T744</f>
         <v>-0.75000000000005684</v>
       </c>
       <c r="V744" s="8"/>

</xml_diff>